<commit_message>
added single cell examples and improvements to deviance computation
</commit_message>
<xml_diff>
--- a/paper2/glm/settings/sequential_predictorSettings.xlsx
+++ b/paper2/glm/settings/sequential_predictorSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Desktop\github\locomotionAnalysis\paper2\glm\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC953688-67DB-4342-B399-8FCDDD497F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C51EC5-F7C4-4F9F-AF93-137513ED77E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="7500" windowHeight="6000" xr2:uid="{4669D966-A741-4C3C-B919-B304607B653B}"/>
+    <workbookView xWindow="-3645" yWindow="13170" windowWidth="7500" windowHeight="6000" activeTab="1" xr2:uid="{4669D966-A741-4C3C-B919-B304607B653B}"/>
   </bookViews>
   <sheets>
     <sheet name="predictors" sheetId="1" r:id="rId1"/>
@@ -40,31 +40,7 @@
     <author>Richard Warren</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{B0AFD67C-9992-48F5-8A75-31400D4766EC}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Richard Warren:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-space separated list of predictor groups to be 'explained away' before building models using this group // use to determine how much unique deviance is explained bythe predictor group</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{BD4FA76A-1DF2-48CA-84D4-6AA08633DFA7}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{BD4FA76A-1DF2-48CA-84D4-6AA08633DFA7}">
       <text>
         <r>
           <rPr>
@@ -90,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{C414666D-4F33-4C6F-A929-76E8B3D0F707}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{C414666D-4F33-4C6F-A929-76E8B3D0F707}">
       <text>
         <r>
           <rPr>
@@ -120,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
   <si>
     <t>name</t>
   </si>
@@ -146,15 +122,9 @@
     <t>group</t>
   </si>
   <si>
-    <t>residuals</t>
-  </si>
-  <si>
     <t>velocity</t>
   </si>
   <si>
-    <t>grossKinematics</t>
-  </si>
-  <si>
     <t>bodyAngle</t>
   </si>
   <si>
@@ -173,9 +143,6 @@
     <t>paw1LH_x</t>
   </si>
   <si>
-    <t>pawKinematics</t>
-  </si>
-  <si>
     <t>paw2LF_x</t>
   </si>
   <si>
@@ -251,9 +218,6 @@
     <t>whiskerAngle</t>
   </si>
   <si>
-    <t>whiskers</t>
-  </si>
-  <si>
     <t>whiskerContact</t>
   </si>
   <si>
@@ -266,43 +230,40 @@
     <t>ear_vel</t>
   </si>
   <si>
-    <t>face</t>
-  </si>
-  <si>
     <t>nose_vel</t>
   </si>
   <si>
     <t>obsToWisk</t>
   </si>
   <si>
-    <t>obstacle</t>
-  </si>
-  <si>
     <t>light</t>
   </si>
   <si>
-    <t>vision</t>
-  </si>
-  <si>
     <t>reward_normal</t>
   </si>
   <si>
-    <t>reward</t>
-  </si>
-  <si>
-    <t>restrict_time</t>
-  </si>
-  <si>
-    <t>obstacle grossKinematics</t>
-  </si>
-  <si>
-    <t>noseVel</t>
-  </si>
-  <si>
-    <t>response</t>
-  </si>
-  <si>
     <t>lickRate</t>
+  </si>
+  <si>
+    <t>phase</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>finekin</t>
+  </si>
+  <si>
+    <t>finekinematics</t>
+  </si>
+  <si>
+    <t>fine_kinematics</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>model with predictors similar to those used in "Cerebellar Contribution to Preparatory Activity in Motor Neocortex"</t>
   </si>
 </sst>
 </file>
@@ -699,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E69B2E9-D98C-4615-9F0D-8BE0A12B27A9}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +701,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>0.25</v>
@@ -749,12 +710,12 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>0.25</v>
@@ -763,12 +724,12 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>0.25</v>
@@ -777,12 +738,12 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F5">
         <v>0.25</v>
@@ -791,12 +752,12 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>0.25</v>
@@ -805,12 +766,12 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F7">
         <v>0.25</v>
@@ -819,276 +780,276 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G26">
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D32">
         <v>8</v>
@@ -1100,23 +1061,23 @@
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1131,45 +1092,45 @@
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D38">
         <v>8</v>
@@ -1181,12 +1142,12 @@
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D39">
         <v>8</v>
@@ -1203,7 +1164,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1218,12 +1179,12 @@
         <v>1</v>
       </c>
       <c r="H40" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>-0.1</v>
@@ -1238,18 +1199,33 @@
         <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G42">
         <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>46</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1260,123 +1236,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B999F951-502D-4BBA-A1C1-34CC8D7DAA2C}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" t="s">
         <v>52</v>
-      </c>
-      <c r="D8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding plots for figure 2
</commit_message>
<xml_diff>
--- a/paper2/glm/settings/sequential_predictorSettings.xlsx
+++ b/paper2/glm/settings/sequential_predictorSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Desktop\github\locomotionAnalysis\paper2\glm\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C51EC5-F7C4-4F9F-AF93-137513ED77E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDCF65E-16B6-42B6-BAAD-E1CBC4BEC6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3645" yWindow="13170" windowWidth="7500" windowHeight="6000" activeTab="1" xr2:uid="{4669D966-A741-4C3C-B919-B304607B653B}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15885" xr2:uid="{4669D966-A741-4C3C-B919-B304607B653B}"/>
   </bookViews>
   <sheets>
     <sheet name="predictors" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
   <si>
     <t>name</t>
   </si>
@@ -249,9 +249,6 @@
   </si>
   <si>
     <t>base</t>
-  </si>
-  <si>
-    <t>finekin</t>
   </si>
   <si>
     <t>finekinematics</t>
@@ -660,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E69B2E9-D98C-4615-9F0D-8BE0A12B27A9}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,7 +721,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -738,7 +735,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -752,7 +749,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -766,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -791,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -802,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -813,7 +810,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -824,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -835,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -846,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -857,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -868,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -879,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -890,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -901,7 +898,7 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -912,7 +909,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -923,7 +920,7 @@
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -934,7 +931,7 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -945,7 +942,7 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -956,7 +953,7 @@
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -967,7 +964,7 @@
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -978,7 +975,7 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -989,7 +986,7 @@
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1000,7 +997,7 @@
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1011,7 +1008,7 @@
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1022,7 +1019,7 @@
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1033,7 +1030,7 @@
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1044,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1072,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1092,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1103,7 +1100,7 @@
         <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1114,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="H36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1125,7 +1122,7 @@
         <v>0</v>
       </c>
       <c r="H37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1142,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1159,7 +1156,7 @@
         <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1211,21 +1208,6 @@
       </c>
       <c r="H42" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E50" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E51" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E52" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1238,7 +1220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B999F951-502D-4BBA-A1C1-34CC8D7DAA2C}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1254,7 +1236,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,7 +1244,7 @@
         <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1272,7 +1254,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>